<commit_message>
avance spacy y selectores
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -1,37 +1,290 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcastillo.ext\Documents\FARMATODO COGIDO\ALGOLIA\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Gluten Free</t>
+  </si>
+  <si>
+    <t>Sugar Free</t>
+  </si>
+  <si>
+    <t>Talla</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>Tipo de piel</t>
+  </si>
+  <si>
+    <t>Tipo de cabello</t>
+  </si>
+  <si>
+    <t>Tono / Color</t>
+  </si>
+  <si>
+    <t>Acabado</t>
+  </si>
+  <si>
+    <t>Cobertura</t>
+  </si>
+  <si>
+    <t>Formato cosmético</t>
+  </si>
+  <si>
+    <t>Función / Beneficio</t>
+  </si>
+  <si>
+    <t>Duración / Resistencia al agua</t>
+  </si>
+  <si>
+    <t>Con fragancia (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con protección solar (Sí / No)</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>Ingredientes activos</t>
+  </si>
+  <si>
+    <t>Edad recomendada / Etapa bebé</t>
+  </si>
+  <si>
+    <t>Formato bebé</t>
+  </si>
+  <si>
+    <t>Hipoalergénico / Dermatológicamente probado (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con ingredientes naturales (Sí / No)</t>
+  </si>
+  <si>
+    <t>Sin conservantes (Sí / No)</t>
+  </si>
+  <si>
+    <t>Material / Textura bebé</t>
+  </si>
+  <si>
+    <t>Antiderrames / Anticólicos / Antibacteriano (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con BPA (Sí / No)</t>
+  </si>
+  <si>
+    <t>Compatible con esterilizadores (Sí / No)</t>
+  </si>
+  <si>
+    <t>Facilidad de digestión (Sí / No / Alta / Media / Baja)</t>
+  </si>
+  <si>
+    <t>Con alcohol (Sí / No)</t>
+  </si>
+  <si>
+    <t>Protección 24h / Resistente al agua (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con color (Sí / No)</t>
+  </si>
+  <si>
+    <t>Zonas de uso</t>
+  </si>
+  <si>
+    <t>Libre de alcohol (Sí / No)</t>
+  </si>
+  <si>
+    <t>Libre de aceites (Sí / No)</t>
+  </si>
+  <si>
+    <t>Libre de parabenos (Sí / No)</t>
+  </si>
+  <si>
+    <t>Libre de comedogénicos (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con enjuague (Sí / No)</t>
+  </si>
+  <si>
+    <t>Orgánico (Sí / No)</t>
+  </si>
+  <si>
+    <t>Natural (Sí / No)</t>
+  </si>
+  <si>
+    <t>Sin aditivos (Sí / No)</t>
+  </si>
+  <si>
+    <t>Vegetariano (Sí / No)</t>
+  </si>
+  <si>
+    <t>Keto (Sí / No)</t>
+  </si>
+  <si>
+    <t>Bajo en sodio (Sí / No)</t>
+  </si>
+  <si>
+    <t>Fuente de proteína (Sí / No)</t>
+  </si>
+  <si>
+    <t>Fuente de fibra (Sí / No)</t>
+  </si>
+  <si>
+    <t>Fuente de vitaminas (Sí / No)</t>
+  </si>
+  <si>
+    <t>Apto para diabéticos (Sí / No)</t>
+  </si>
+  <si>
+    <t>Apto para celíacos (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con edulcorantes naturales (Sí / No)</t>
+  </si>
+  <si>
+    <t>Con edulcorantes artificiales (Sí / No)</t>
+  </si>
+  <si>
+    <t>Función hogar</t>
+  </si>
+  <si>
+    <t>Fragancia hogar</t>
+  </si>
+  <si>
+    <t>Biodegradable (Sí / No)</t>
+  </si>
+  <si>
+    <t>Reutilizable (Sí / No)</t>
+  </si>
+  <si>
+    <t>Compatible con lavavajillas / microondas / mascotas / superficies</t>
+  </si>
+  <si>
+    <t>Durabilidad / Resistencia</t>
+  </si>
+  <si>
+    <t>Uso (Interior / Exterior)</t>
+  </si>
+  <si>
+    <t>Sabor o aroma (para mascotas o alimentos)</t>
+  </si>
+  <si>
+    <t>Beneficio para mascotas</t>
+  </si>
+  <si>
+    <t>Tipo de suplemento</t>
+  </si>
+  <si>
+    <t>Objetivo / Beneficio deportivo</t>
+  </si>
+  <si>
+    <t>Sabor deportivo</t>
+  </si>
+  <si>
+    <t>Presentación suplemento</t>
+  </si>
+  <si>
+    <t>Con cafeína (Sí / No)</t>
+  </si>
+  <si>
+    <t>Sin lactosa (Sí / No)</t>
+  </si>
+  <si>
+    <t>Certificaciones</t>
+  </si>
+  <si>
+    <t>Forma de consumo</t>
+  </si>
+  <si>
+    <t>Incluye accesorios (Sí / No)</t>
+  </si>
+  <si>
+    <t>Tipo de deporte</t>
+  </si>
+  <si>
+    <t>Compatibilidad con apps, máquinas o rutinas (Sí / No)</t>
+  </si>
+  <si>
+    <t>1001539</t>
+  </si>
+  <si>
+    <t>Ureaderm Loción Frasco X225g. Med Urea Ácido Láctico</t>
+  </si>
+  <si>
+    <t>$150.400</t>
+  </si>
+  <si>
+    <t>1001578</t>
+  </si>
+  <si>
+    <t>Shampoo Novaderma Octodir Elimina Seborrea X120ml.</t>
+  </si>
+  <si>
+    <t>$85.750</t>
+  </si>
+  <si>
+    <t>1001634</t>
+  </si>
+  <si>
+    <t>Gel Benzac Ac 5 Porciento Limpiador Contra El Acné X60g</t>
+  </si>
+  <si>
+    <t>$58.475</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +299,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,105 +623,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BT5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Precio</t>
-        </is>
+    <row r="1" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1001038</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Tiras Freestyle Optium Glucómetro X 25 Und</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>$82.950</t>
-        </is>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1031657</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1001539</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ureaderm Loción Frasco X225g. Med Urea Ácido Láctico</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$150.400</t>
-        </is>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1001578</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Shampoo Novaderma Octodir Elimina Seborrea X120ml.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$85.750</t>
-        </is>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1001634</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Gel Benzac Ac 5 Porciento Limpiador Contra El Acné X60g</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>$58.475</t>
-        </is>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>